<commit_message>
Change the spelling to -Expenses
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,73 +415,51 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Food</v>
+        <v>Gym Monthly</v>
       </c>
       <c r="B2">
-        <v>12.5</v>
+        <v>800</v>
       </c>
       <c r="C2" t="str">
-        <v>2025-11-23T00:00:00.000Z</v>
+        <v>2025-11-30T00:00:00.000Z</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Groceries</v>
+        <v>New Clothes</v>
       </c>
       <c r="B3">
         <v>500</v>
       </c>
       <c r="C3" t="str">
-        <v>2025-11-22T00:00:00.000Z</v>
+        <v>2025-11-20T00:00:00.000Z</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Load</v>
+        <v>Groceries</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>2000</v>
       </c>
       <c r="C4" t="str">
-        <v>2025-11-21T00:00:00.000Z</v>
+        <v>2025-11-16T00:00:00.000Z</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Snacks</v>
+        <v>House Rent</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>5000</v>
       </c>
       <c r="C5" t="str">
-        <v>2025-11-11T00:00:00.000Z</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Travel</v>
-      </c>
-      <c r="B6">
-        <v>580</v>
-      </c>
-      <c r="C6" t="str">
-        <v>2025-11-06T00:00:00.000Z</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Rent</v>
-      </c>
-      <c r="B7">
-        <v>5000</v>
-      </c>
-      <c r="C7" t="str">
-        <v>2025-11-02T00:00:00.000Z</v>
+        <v>2025-11-15T00:00:00.000Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>